<commit_message>
Added modified files for RFP
</commit_message>
<xml_diff>
--- a/EvRefApp6/EV/Results/P1/ConsumptionValues.xlsx
+++ b/EvRefApp6/EV/Results/P1/ConsumptionValues.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\UWAFT\Competition\EvRefApp6\EV\Results\P1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\UWAFT\RFP-CSMS\EvRefApp6\EV\Results\P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>HWFET</t>
   </si>
@@ -45,6 +45,48 @@
   </si>
   <si>
     <t>ACC_2 Energy Consumption (Wh/mi) 2m Gap</t>
+  </si>
+  <si>
+    <t>Drive Cycle</t>
+  </si>
+  <si>
+    <t>BattDisEnrgyTotal ACC Wh</t>
+  </si>
+  <si>
+    <t>BattRegEnrgyTotal ACC Wh</t>
+  </si>
+  <si>
+    <t>BattDisEnrgyTotal NACC Wh</t>
+  </si>
+  <si>
+    <t>BattRegEnrgyTotal NACC Wh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BattDisEnrgyTotal </t>
+  </si>
+  <si>
+    <t>BattRegEnrgyTotal</t>
+  </si>
+  <si>
+    <t>Non ACC</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>Total Energy Consumption</t>
+  </si>
+  <si>
+    <t>WOT</t>
+  </si>
+  <si>
+    <t>BattDisEnrgy Per Event</t>
+  </si>
+  <si>
+    <t>BattRegEnrgyTotal Per Event</t>
+  </si>
+  <si>
+    <t>Total Energy Consumption Per event</t>
   </si>
 </sst>
 </file>
@@ -80,8 +122,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,9 +451,16 @@
     <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -423,59 +473,237 @@
       <c r="E1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>122.0938</v>
+        <v>204.89259999999999</v>
       </c>
       <c r="C2">
-        <v>121.9919</v>
+        <v>204.7423</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D3" si="0">B2-C2</f>
-        <v>0.10190000000000055</v>
+        <v>0.15029999999998722</v>
       </c>
       <c r="E2">
-        <v>121.9187</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204.56829999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2255.1999999999998</v>
+      </c>
+      <c r="G2" s="1">
+        <v>162.23099999999999</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2232.6</v>
+      </c>
+      <c r="I2" s="1">
+        <v>140.1337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>105.288</v>
+        <v>178.1069</v>
       </c>
       <c r="C3">
-        <v>104.4534</v>
+        <v>176.6885</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>0.83459999999999468</v>
+        <v>1.4183999999999912</v>
       </c>
       <c r="E3">
-        <v>104.4666</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>175.77449999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1717.8</v>
+      </c>
+      <c r="G3" s="1">
+        <v>401.03030000000001</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1683</v>
+      </c>
+      <c r="I3" s="1">
+        <v>374.91039999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>164.75299999999999</v>
+        <v>274.64490000000001</v>
       </c>
       <c r="C4">
-        <v>164.3492</v>
+        <v>274.31979999999999</v>
       </c>
       <c r="D4">
         <f>B4-C4</f>
-        <v>0.40379999999998972</v>
+        <v>0.32510000000002037</v>
       </c>
       <c r="E4">
-        <v>164.28540000000001</v>
+        <v>273.07990000000001</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2762.6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>575.33810000000005</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2700.8</v>
+      </c>
+      <c r="I4" s="1">
+        <v>512.99760000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>325.92989999999998</v>
+      </c>
+      <c r="C7">
+        <v>180.0763</v>
+      </c>
+      <c r="D7">
+        <f>B7-C7</f>
+        <v>145.85359999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>314.33999999999997</v>
+      </c>
+      <c r="C8">
+        <v>176.43129999999999</v>
+      </c>
+      <c r="D8">
+        <f>B8-C8</f>
+        <v>137.90869999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>336.04390000000001</v>
+      </c>
+      <c r="C11">
+        <v>100.8359</v>
+      </c>
+      <c r="D11">
+        <f>B11-C11</f>
+        <v>235.20800000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>325.53609999999998</v>
+      </c>
+      <c r="C12">
+        <v>96.105500000000006</v>
+      </c>
+      <c r="D12">
+        <f>B12-C12</f>
+        <v>229.43059999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>322.11500000000001</v>
+      </c>
+      <c r="C13">
+        <v>95.179000000000002</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:D15" si="1">B13-C13</f>
+        <v>226.93600000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>320.4556</v>
+      </c>
+      <c r="C14">
+        <v>95.211200000000005</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>225.24439999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>319.5206</v>
+      </c>
+      <c r="C15">
+        <v>95.635800000000003</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>223.88479999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>